<commit_message>
Update in answer key file
</commit_message>
<xml_diff>
--- a/poll_answers/CSE3063_20201123_Mon_zoom_PollAnswerKey.xlsx
+++ b/poll_answers/CSE3063_20201123_Mon_zoom_PollAnswerKey.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Boş İşler\ÜNİVERSİTE\Object Oriented Software Design\Proje 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berky\CSE3063F20P2_GRP7\poll_answers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A136CDE8-9924-4720-AE38-D5F50E809311}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D38CC3-3452-464B-8E4E-677C2AF17412}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="3216" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>CSE3063_20201123_Mon_zoom_Poll</t>
-  </si>
-  <si>
-    <t>Answer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Question </t>
   </si>
   <si>
     <t>How do you model the following situation with a UML class diagram: A season worker may be employed in one or several 
@@ -101,19 +95,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3C4043"/>
-      <name val="Calibri "/>
-      <charset val="162"/>
     </font>
   </fonts>
   <fills count="2">
@@ -136,9 +124,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -422,39 +409,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="90.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A3" s="2" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -462,7 +449,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -470,7 +457,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -478,7 +465,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -486,7 +473,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -494,7 +481,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -502,7 +489,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -510,20 +497,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="14.4" customHeight="1">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>19</v>
       </c>
       <c r="B11" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>